<commit_message>
optimise the gsc add girl voice
</commit_message>
<xml_diff>
--- a/snr.xlsx
+++ b/snr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>噪声源</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -169,6 +169,86 @@
   </si>
   <si>
     <t xml:space="preserve">滤波器阶数：32 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fwiener-GSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-7.72</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.70</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.97</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.89</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-5.81</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-3.14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.73</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAD-Wiener-GSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.73</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -536,9 +616,10 @@
     <col min="4" max="4" width="14" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -546,8 +627,10 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -563,9 +646,14 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -581,8 +669,14 @@
       <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -598,8 +692,14 @@
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -615,8 +715,14 @@
       <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -632,8 +738,14 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -649,8 +761,14 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -666,8 +784,14 @@
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -683,8 +807,14 @@
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -700,8 +830,14 @@
       <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -716,6 +852,12 @@
       </c>
       <c r="E11" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>